<commit_message>
Fixed bug in python script. Also refactored a bit
</commit_message>
<xml_diff>
--- a/mongodbInsertScript/placeWholesaleExcelFileHere/z_sampleExcelForScript.xlsx
+++ b/mongodbInsertScript/placeWholesaleExcelFileHere/z_sampleExcelForScript.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeePhan\Desktop\inventory-manager\mongodbInsertScript\placeWholesaleExcelFileHere\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6882B8-5E49-48C7-9874-66AEA9455BC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="16275" windowHeight="9780"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wholesale#1" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>UPC</t>
   </si>
@@ -135,12 +141,15 @@
   </si>
   <si>
     <t>zProd9</t>
+  </si>
+  <si>
+    <t>Preparation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,7 +237,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="38">
     <dxf>
@@ -537,66 +546,66 @@
     </dxf>
   </dxfs>
   <tableStyles count="13" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Template-style" pivot="0" count="3">
+    <tableStyle name="Template-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="37"/>
       <tableStyleElement type="firstRowStripe" dxfId="36"/>
       <tableStyleElement type="secondRowStripe" dxfId="35"/>
     </tableStyle>
-    <tableStyle name="Template-style 2" pivot="0" count="3">
+    <tableStyle name="Template-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="34"/>
       <tableStyleElement type="firstRowStripe" dxfId="33"/>
       <tableStyleElement type="secondRowStripe" dxfId="32"/>
     </tableStyle>
-    <tableStyle name="Gemini-style" pivot="0" count="3">
+    <tableStyle name="Gemini-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
       <tableStyleElement type="headerRow" dxfId="31"/>
       <tableStyleElement type="firstRowStripe" dxfId="30"/>
       <tableStyleElement type="secondRowStripe" dxfId="29"/>
     </tableStyle>
-    <tableStyle name="Gemini-style 2" pivot="0" count="3">
+    <tableStyle name="Gemini-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
       <tableStyleElement type="headerRow" dxfId="28"/>
       <tableStyleElement type="firstRowStripe" dxfId="27"/>
       <tableStyleElement type="secondRowStripe" dxfId="26"/>
     </tableStyle>
-    <tableStyle name="Kim Seng -style" pivot="0" count="3">
+    <tableStyle name="Kim Seng -style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
       <tableStyleElement type="headerRow" dxfId="25"/>
       <tableStyleElement type="firstRowStripe" dxfId="24"/>
       <tableStyleElement type="secondRowStripe" dxfId="23"/>
     </tableStyle>
-    <tableStyle name="Kim Seng -style 2" pivot="0" count="3">
+    <tableStyle name="Kim Seng -style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
       <tableStyleElement type="headerRow" dxfId="22"/>
       <tableStyleElement type="firstRowStripe" dxfId="21"/>
       <tableStyleElement type="secondRowStripe" dxfId="20"/>
     </tableStyle>
-    <tableStyle name="Kim Seng -style 3" pivot="0" count="2">
+    <tableStyle name="Kim Seng -style 3" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
       <tableStyleElement type="firstRowStripe" dxfId="19"/>
       <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
-    <tableStyle name="Kanboo-style" pivot="0" count="3">
+    <tableStyle name="Kanboo-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
       <tableStyleElement type="headerRow" dxfId="17"/>
       <tableStyleElement type="firstRowStripe" dxfId="16"/>
       <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
-    <tableStyle name="K &amp; M Trading-style" pivot="0" count="3">
+    <tableStyle name="K &amp; M Trading-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="firstRowStripe" dxfId="13"/>
       <tableStyleElement type="secondRowStripe" dxfId="12"/>
     </tableStyle>
-    <tableStyle name="K &amp; M Trading-style 2" pivot="0" count="3">
+    <tableStyle name="K &amp; M Trading-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
       <tableStyleElement type="headerRow" dxfId="11"/>
       <tableStyleElement type="firstRowStripe" dxfId="10"/>
       <tableStyleElement type="secondRowStripe" dxfId="9"/>
     </tableStyle>
-    <tableStyle name="Empire-style" pivot="0" count="3">
+    <tableStyle name="Empire-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0A000000}">
       <tableStyleElement type="headerRow" dxfId="8"/>
       <tableStyleElement type="firstRowStripe" dxfId="7"/>
       <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
-    <tableStyle name="AsianFoodGrocer-style" pivot="0" count="3">
+    <tableStyle name="AsianFoodGrocer-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0B000000}">
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="firstRowStripe" dxfId="4"/>
       <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle name="Takari-style" pivot="0" count="3">
+    <tableStyle name="Takari-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0C000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -605,6 +614,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -653,7 +665,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,9 +698,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,6 +750,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -896,30 +942,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="6" customWidth="1"/>
-    <col min="2" max="3" width="17.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="17.7265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12" style="6" customWidth="1"/>
     <col min="6" max="6" width="11" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="7" width="11.54296875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -941,8 +988,11 @@
       <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -965,7 +1015,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -988,7 +1038,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1011,7 +1061,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1040,31 +1090,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="6" customWidth="1"/>
-    <col min="2" max="3" width="17.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="17.7265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12" style="6" customWidth="1"/>
     <col min="6" max="6" width="11" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="7" max="7" width="11.54296875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
@@ -1116,7 +1166,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -1142,7 +1192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1168,7 +1218,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>

</xml_diff>